<commit_message>
add viz to other tabs
</commit_message>
<xml_diff>
--- a/data1.xlsx
+++ b/data1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MSDS\Info Viz\Client Project SOFI\SOFI-2035-Info-Viz-code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5256D051-FDDE-4FB4-BFD0-7D001D2FEE7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F4289A-C1FA-45DB-8387-9A63005576A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{6664DB92-7A09-4C4D-AD27-8941A5E73883}"/>
   </bookViews>
@@ -9641,8 +9641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{517EB363-C416-498A-9193-B8E2F76BE05F}">
   <dimension ref="A1:D1032222"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="I37" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>